<commit_message>
Update script - fix data names.
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_files\git_open\meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C6FCCF-A9F8-46A6-8AAA-5482B8F6DB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD64665B-56F3-4156-857C-6FDF5B5ADD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>